<commit_message>
Added multiple pdf functionality
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,39 +436,46 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Nume</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Prenume</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Data Tiparire</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nume</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Prenume</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Perioada Internarii</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Urgenta</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>04/08/2022</t>
+          <t xml:space="preserve">AFTINIE 
+</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AFTINIE</t>
+          <t xml:space="preserve">GRIGORITA 
+</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GRIGORITA</t>
+          <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -476,6 +483,109 @@
           <t xml:space="preserve">26/11/2019 08:04 - 02/12/2019 10:05 (6 zile) </t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NU 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALIMAN 
+</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOISE 
+</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">04/08/2022 </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">05/12/2019 17:03 - 13/12/2019 12:20 (8 zile) </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DA 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AVRAM 
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IULICA 
+</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">04/08/2022 </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18/11/2019 09:20 - 22/11/2019 13:34 (4 zile) </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NU 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BALASA 
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IOANA 
+</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">04/08/2022 </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">25/11/2019 09:19 - 29/11/2019 12:44 (4 zile) </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NU 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added some fields but errors
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Output" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Output" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Varsta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Data Tiparire</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Perioada Internarii</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Urgenta</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LDL COLESTEROL</t>
         </is>
       </c>
     </row>
@@ -475,20 +485,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t xml:space="preserve">71 ani si 0 luni 
+</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">26/11/2019 08:04 - 02/12/2019 10:05 (6 zile) </t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,20 +522,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t xml:space="preserve">78 ani si 2 luni 
+</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve">05/12/2019 17:03 - 13/12/2019 12:20 (8 zile) </t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t xml:space="preserve">DA 
 </t>
         </is>
       </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -535,20 +559,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t xml:space="preserve">55 ani si 3 luni 
+</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">18/11/2019 09:20 - 22/11/2019 13:34 (4 zile) </t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -565,20 +596,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t xml:space="preserve">67 ani si 1 luni 
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t xml:space="preserve">25/11/2019 09:19 - 29/11/2019 12:44 (4 zile) </t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -595,20 +633,432 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t xml:space="preserve">64 ani si 6 luni 
+</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t xml:space="preserve">04/08/2022 </t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t xml:space="preserve">19/11/2019 08:23 - 22/11/2019 12:45 (3 zile) </t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added more columns and likleyhood search
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Numar zile</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Urgenta</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Hipertensiune</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>LDL COLESTEROL</t>
         </is>
@@ -496,16 +506,30 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">26/11/2019 08:04 - 02/12/2019 10:05 (6 zile) </t>
+          <t>26/11/2019 08:04 - 02/12/2019</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Da</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>97.36000000000001</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -533,16 +557,30 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">05/12/2019 17:03 - 13/12/2019 12:20 (8 zile) </t>
+          <t>05/12/2019 17:03 - 13/12/2019</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t xml:space="preserve">DA 
 </t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Da</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>49.72000000000001</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -570,16 +608,30 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">18/11/2019 09:20 - 22/11/2019 13:34 (4 zile) </t>
+          <t>18/11/2019 09:20 - 22/11/2019</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Da</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>97.44</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -607,16 +659,30 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">25/11/2019 09:19 - 29/11/2019 12:44 (4 zile) </t>
+          <t>25/11/2019 09:19 - 29/11/2019</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Da</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>114.38</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -644,16 +710,30 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">19/11/2019 08:23 - 22/11/2019 12:45 (3 zile) </t>
+          <t>19/11/2019 08:23 - 22/11/2019</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t xml:space="preserve">NU 
 </t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Da</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>93.82</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -663,6 +743,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -672,6 +754,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -681,6 +765,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -690,6 +776,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -699,6 +787,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -708,6 +798,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -717,6 +809,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -726,6 +820,8 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -735,6 +831,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -744,6 +842,8 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -753,6 +853,8 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -762,6 +864,8 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -771,6 +875,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -780,6 +886,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -789,6 +897,8 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -798,6 +908,8 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -807,6 +919,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -816,6 +930,8 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -825,6 +941,8 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -834,6 +952,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -843,6 +963,8 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -852,6 +974,8 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -861,6 +985,8 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -870,6 +996,8 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -879,6 +1007,8 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -888,6 +1018,8 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -897,6 +1029,8 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -906,6 +1040,8 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -915,6 +1051,8 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -924,6 +1062,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -933,6 +1073,8 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
@@ -942,6 +1084,8 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
@@ -951,6 +1095,8 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -960,6 +1106,8 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -969,6 +1117,8 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -978,6 +1128,8 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -987,6 +1139,8 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -996,6 +1150,8 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
@@ -1005,6 +1161,8 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -1014,6 +1172,8 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -1023,6 +1183,8 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -1032,6 +1194,8 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -1041,6 +1205,8 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -1050,6 +1216,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -1059,6 +1227,8 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>